<commit_message>
bom update - print surface 330
</commit_message>
<xml_diff>
--- a/Document Library/Bill Of Materials/Valkyrie BOM Beta 07.xlsx
+++ b/Document Library/Bill Of Materials/Valkyrie BOM Beta 07.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3837cd5b4a1a02ac/Document Library/GitHub/Project-Valkyrie/Document Library/Bill Of Materials/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="11_90E8A2594C63906364F20E90CDD1628CCD4781EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2FD240B4-886A-49AB-963C-BE5BE8159B0B}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="11_90E8A2594C63906364F20E90CDD1628CCD4781EF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8E513DF3-6A01-4569-BE19-6AF3853D6C03}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -703,12 +703,6 @@
     <t>Print Surface</t>
   </si>
   <si>
-    <t>Removal Spring Steel Sheet</t>
-  </si>
-  <si>
-    <t>Size: 310x310mm</t>
-  </si>
-  <si>
     <t>Energetic</t>
   </si>
   <si>
@@ -1532,6 +1526,12 @@
   </si>
   <si>
     <t>Keenovo</t>
+  </si>
+  <si>
+    <t>Size: 330x330mm</t>
+  </si>
+  <si>
+    <t>Removal Spring Steel PEI Sheet</t>
   </si>
 </sst>
 </file>
@@ -1893,7 +1893,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2061,6 +2061,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2627,7 +2628,7 @@
     <row r="2" spans="1:26">
       <c r="A2" s="1"/>
       <c r="B2" s="5" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:26">
@@ -2657,7 +2658,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D8" s="8" t="s">
         <v>6</v>
@@ -2669,7 +2670,7 @@
       <c r="I8" s="9"/>
       <c r="J8" s="63">
         <f>J112</f>
-        <v>1870.85</v>
+        <v>1880.85</v>
       </c>
       <c r="K8" s="8"/>
       <c r="L8" s="10"/>
@@ -2790,7 +2791,7 @@
       <c r="N10" s="74"/>
       <c r="O10" s="53"/>
       <c r="P10" s="85" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="11" spans="1:26">
@@ -2837,7 +2838,7 @@
       <c r="N11" s="75"/>
       <c r="O11" s="54"/>
       <c r="P11" s="85" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="12" spans="1:26">
@@ -2883,7 +2884,7 @@
       <c r="N12" s="75"/>
       <c r="O12" s="54"/>
       <c r="P12" s="85" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="13" spans="1:26">
@@ -2929,7 +2930,7 @@
       <c r="N13" s="75"/>
       <c r="O13" s="54"/>
       <c r="P13" s="85" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="14" spans="1:26">
@@ -2975,7 +2976,7 @@
       <c r="N14" s="75"/>
       <c r="O14" s="54"/>
       <c r="P14" s="85" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="15" spans="1:26">
@@ -3007,7 +3008,7 @@
         <v>25</v>
       </c>
       <c r="K15" s="36" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="L15" s="33" t="s">
         <v>28</v>
@@ -3015,22 +3016,22 @@
       <c r="M15" s="34"/>
       <c r="N15" s="75"/>
       <c r="O15" s="62" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="P15" s="35"/>
     </row>
     <row r="16" spans="1:26">
       <c r="A16" s="26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B16" s="38" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C16" s="38" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D16" s="38" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E16" s="27">
         <v>350</v>
@@ -3050,10 +3051,10 @@
         <v>46.8</v>
       </c>
       <c r="K16" s="32" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="L16" s="33" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M16" s="34"/>
       <c r="N16" s="75"/>
@@ -3062,16 +3063,16 @@
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B17" s="38" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C17" s="38" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D17" s="38" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E17" s="27">
         <v>400</v>
@@ -3091,10 +3092,10 @@
         <v>35</v>
       </c>
       <c r="K17" s="36" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="L17" s="33" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M17" s="40"/>
       <c r="N17" s="76"/>
@@ -3103,16 +3104,16 @@
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B18" s="38" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C18" s="38" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D18" s="38" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E18" s="27">
         <v>400</v>
@@ -3132,10 +3133,10 @@
         <v>16</v>
       </c>
       <c r="K18" s="36" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="L18" s="33" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M18" s="34"/>
       <c r="N18" s="75"/>
@@ -3153,7 +3154,7 @@
         <v>39</v>
       </c>
       <c r="D19" s="79" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E19" s="78"/>
       <c r="F19" s="78"/>
@@ -3170,10 +3171,10 @@
         <v>265.60000000000002</v>
       </c>
       <c r="K19" s="97" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="L19" s="82" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="M19" s="83"/>
       <c r="N19" s="84"/>
@@ -3274,31 +3275,31 @@
       <c r="C22" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="D22" s="27" t="s">
-        <v>50</v>
+      <c r="D22" s="99" t="s">
+        <v>315</v>
       </c>
       <c r="E22" s="27">
-        <v>310</v>
+        <v>330</v>
       </c>
       <c r="F22" s="30"/>
       <c r="G22" s="30">
         <v>1</v>
       </c>
       <c r="H22" s="31">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="I22" s="30">
         <v>1</v>
       </c>
       <c r="J22" s="31">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="K22" s="32" t="s">
-        <v>51</v>
+        <v>314</v>
       </c>
       <c r="L22" s="33" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="M22" s="34"/>
       <c r="N22" s="34"/>
@@ -3307,16 +3308,16 @@
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B23" s="27" t="s">
         <v>24</v>
       </c>
       <c r="C23" s="27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D23" s="38" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E23" s="27">
         <v>25</v>
@@ -3336,10 +3337,10 @@
         <v>1.2</v>
       </c>
       <c r="K23" s="36" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="L23" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M23" s="34"/>
       <c r="N23" s="34"/>
@@ -3348,16 +3349,16 @@
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B24" s="27" t="s">
         <v>24</v>
       </c>
       <c r="C24" s="27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D24" s="27" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E24" s="27">
         <v>40</v>
@@ -3377,10 +3378,10 @@
         <v>9</v>
       </c>
       <c r="K24" s="32" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="L24" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M24" s="34"/>
       <c r="N24" s="34"/>
@@ -3395,10 +3396,10 @@
         <v>24</v>
       </c>
       <c r="C25" s="27" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D25" s="27" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E25" s="27">
         <v>50</v>
@@ -3418,10 +3419,10 @@
         <v>6</v>
       </c>
       <c r="K25" s="36" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L25" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M25" s="34"/>
       <c r="N25" s="34"/>
@@ -3436,10 +3437,10 @@
         <v>24</v>
       </c>
       <c r="C26" s="27" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D26" s="27" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E26" s="27"/>
       <c r="F26" s="30"/>
@@ -3457,10 +3458,10 @@
         <v>3</v>
       </c>
       <c r="K26" s="32" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="L26" s="33" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="M26" s="34"/>
       <c r="N26" s="34"/>
@@ -3475,10 +3476,10 @@
         <v>24</v>
       </c>
       <c r="C27" s="27" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D27" s="27" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E27" s="27">
         <v>30</v>
@@ -3498,10 +3499,10 @@
         <v>5</v>
       </c>
       <c r="K27" s="36" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L27" s="33" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M27" s="34"/>
       <c r="N27" s="34"/>
@@ -3510,16 +3511,16 @@
     </row>
     <row r="28" spans="1:16">
       <c r="A28" s="26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B28" s="27" t="s">
         <v>24</v>
       </c>
       <c r="C28" s="27" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D28" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E28" s="27"/>
       <c r="F28" s="30"/>
@@ -3537,10 +3538,10 @@
         <v>7.5</v>
       </c>
       <c r="K28" s="32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="L28" s="33" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="M28" s="34"/>
       <c r="N28" s="34"/>
@@ -3552,13 +3553,13 @@
         <v>23</v>
       </c>
       <c r="B29" s="27" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="27" t="s">
         <v>74</v>
-      </c>
-      <c r="C29" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="D29" s="27" t="s">
-        <v>76</v>
       </c>
       <c r="E29" s="27"/>
       <c r="F29" s="30"/>
@@ -3576,10 +3577,10 @@
         <v>1</v>
       </c>
       <c r="K29" s="36" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="L29" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M29" s="40">
         <v>934</v>
@@ -3595,13 +3596,13 @@
         <v>23</v>
       </c>
       <c r="B30" s="27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C30" s="27" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D30" s="27" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E30" s="27"/>
       <c r="F30" s="30"/>
@@ -3619,10 +3620,10 @@
         <v>3</v>
       </c>
       <c r="K30" s="36" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="L30" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M30" s="34"/>
       <c r="N30" s="34"/>
@@ -3634,13 +3635,13 @@
         <v>23</v>
       </c>
       <c r="B31" s="27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C31" s="27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D31" s="27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E31" s="27"/>
       <c r="F31" s="30"/>
@@ -3658,10 +3659,10 @@
         <v>1</v>
       </c>
       <c r="K31" s="36" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="L31" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M31" s="40"/>
       <c r="N31" s="40">
@@ -3675,13 +3676,13 @@
         <v>23</v>
       </c>
       <c r="B32" s="27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C32" s="27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D32" s="27" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E32" s="27"/>
       <c r="F32" s="30"/>
@@ -3699,10 +3700,10 @@
         <v>1</v>
       </c>
       <c r="K32" s="32" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="L32" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M32" s="34">
         <v>912</v>
@@ -3716,13 +3717,13 @@
         <v>23</v>
       </c>
       <c r="B33" s="27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C33" s="27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D33" s="27" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E33" s="27"/>
       <c r="F33" s="30"/>
@@ -3740,10 +3741,10 @@
         <v>1</v>
       </c>
       <c r="K33" s="36" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="L33" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M33" s="40"/>
       <c r="N33" s="40">
@@ -3757,13 +3758,13 @@
         <v>23</v>
       </c>
       <c r="B34" s="27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C34" s="27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D34" s="38" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E34" s="27"/>
       <c r="F34" s="30"/>
@@ -3781,10 +3782,10 @@
         <v>2</v>
       </c>
       <c r="K34" s="32" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="L34" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M34" s="34"/>
       <c r="N34" s="34">
@@ -3798,13 +3799,13 @@
         <v>23</v>
       </c>
       <c r="B35" s="27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C35" s="27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D35" s="27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E35" s="27"/>
       <c r="F35" s="30"/>
@@ -3822,10 +3823,10 @@
         <v>12</v>
       </c>
       <c r="K35" s="36" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="L35" s="33" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="M35" s="40"/>
       <c r="N35" s="40"/>
@@ -3837,13 +3838,13 @@
         <v>23</v>
       </c>
       <c r="B36" s="27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C36" s="27" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D36" s="27" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E36" s="27"/>
       <c r="F36" s="30"/>
@@ -3861,10 +3862,10 @@
         <v>1.5</v>
       </c>
       <c r="K36" s="36" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="L36" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M36" s="34">
         <v>934</v>
@@ -3880,13 +3881,13 @@
         <v>23</v>
       </c>
       <c r="B37" s="27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C37" s="27" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D37" s="27" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E37" s="27"/>
       <c r="F37" s="30"/>
@@ -3904,10 +3905,10 @@
         <v>1.5</v>
       </c>
       <c r="K37" s="36" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="L37" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M37" s="40">
         <v>985</v>
@@ -3923,13 +3924,13 @@
         <v>23</v>
       </c>
       <c r="B38" s="27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C38" s="27" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D38" s="27" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E38" s="27"/>
       <c r="F38" s="30"/>
@@ -3947,10 +3948,10 @@
         <v>1</v>
       </c>
       <c r="K38" s="32" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L38" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M38" s="34">
         <v>125</v>
@@ -3966,13 +3967,13 @@
         <v>23</v>
       </c>
       <c r="B39" s="27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C39" s="27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D39" s="38" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E39" s="27"/>
       <c r="F39" s="30"/>
@@ -3990,10 +3991,10 @@
         <v>2</v>
       </c>
       <c r="K39" s="36" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="L39" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M39" s="40"/>
       <c r="N39" s="40">
@@ -4007,13 +4008,13 @@
         <v>23</v>
       </c>
       <c r="B40" s="27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C40" s="27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D40" s="27" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E40" s="27"/>
       <c r="F40" s="30"/>
@@ -4031,10 +4032,10 @@
         <v>2</v>
       </c>
       <c r="K40" s="32" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="L40" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M40" s="34"/>
       <c r="N40" s="34">
@@ -4048,13 +4049,13 @@
         <v>23</v>
       </c>
       <c r="B41" s="27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C41" s="27" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D41" s="27" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E41" s="27"/>
       <c r="F41" s="30"/>
@@ -4072,10 +4073,10 @@
         <v>2</v>
       </c>
       <c r="K41" s="36" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="L41" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M41" s="40">
         <v>934</v>
@@ -4091,13 +4092,13 @@
         <v>23</v>
       </c>
       <c r="B42" s="27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C42" s="27" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E42" s="27"/>
       <c r="F42" s="30"/>
@@ -4115,10 +4116,10 @@
         <v>11</v>
       </c>
       <c r="K42" s="36" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="L42" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M42" s="34"/>
       <c r="N42" s="34"/>
@@ -4130,13 +4131,13 @@
         <v>23</v>
       </c>
       <c r="B43" s="27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C43" s="27" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D43" s="27" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E43" s="27"/>
       <c r="F43" s="30"/>
@@ -4154,10 +4155,10 @@
         <v>2.81</v>
       </c>
       <c r="K43" s="36" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="L43" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M43" s="40">
         <v>985</v>
@@ -4173,13 +4174,13 @@
         <v>23</v>
       </c>
       <c r="B44" s="27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C44" s="27" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D44" s="27" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E44" s="27"/>
       <c r="F44" s="30"/>
@@ -4197,10 +4198,10 @@
         <v>13.5</v>
       </c>
       <c r="K44" s="32" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L44" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M44" s="34"/>
       <c r="N44" s="34"/>
@@ -4212,13 +4213,13 @@
         <v>23</v>
       </c>
       <c r="B45" s="27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C45" s="27" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D45" s="27" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E45" s="27"/>
       <c r="F45" s="30"/>
@@ -4236,10 +4237,10 @@
         <v>2.56</v>
       </c>
       <c r="K45" s="36" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="L45" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M45" s="40">
         <v>125</v>
@@ -4255,13 +4256,13 @@
         <v>23</v>
       </c>
       <c r="B46" s="27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C46" s="27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D46" s="27" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E46" s="27"/>
       <c r="F46" s="30"/>
@@ -4279,10 +4280,10 @@
         <v>32.28</v>
       </c>
       <c r="K46" s="32" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="L46" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M46" s="34"/>
       <c r="N46" s="34">
@@ -4296,13 +4297,13 @@
         <v>23</v>
       </c>
       <c r="B47" s="27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C47" s="27" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D47" s="27" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E47" s="27"/>
       <c r="F47" s="30"/>
@@ -4320,10 +4321,10 @@
         <v>8</v>
       </c>
       <c r="K47" s="36" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="L47" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M47" s="40"/>
       <c r="N47" s="40">
@@ -4337,13 +4338,13 @@
         <v>23</v>
       </c>
       <c r="B48" s="27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C48" s="27" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D48" s="27" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E48" s="27"/>
       <c r="F48" s="30"/>
@@ -4361,10 +4362,10 @@
         <v>2.57</v>
       </c>
       <c r="K48" s="36" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L48" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M48" s="34">
         <v>933</v>
@@ -4380,13 +4381,13 @@
         <v>23</v>
       </c>
       <c r="B49" s="43" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C49" s="43" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D49" s="38" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E49" s="27"/>
       <c r="F49" s="30"/>
@@ -4404,10 +4405,10 @@
         <v>16</v>
       </c>
       <c r="K49" s="36" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="L49" s="33" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="M49" s="40"/>
       <c r="N49" s="40"/>
@@ -4416,16 +4417,16 @@
     </row>
     <row r="50" spans="1:16" s="88" customFormat="1">
       <c r="A50" s="86" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B50" s="87" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C50" s="87" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D50" s="88" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="F50" s="89"/>
       <c r="G50" s="89"/>
@@ -4440,10 +4441,10 @@
         <v>8</v>
       </c>
       <c r="K50" s="36" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="L50" s="92" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M50" s="93"/>
       <c r="N50" s="93"/>
@@ -4455,13 +4456,13 @@
         <v>23</v>
       </c>
       <c r="B51" s="87" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C51" s="88" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D51" s="88" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="F51" s="89"/>
       <c r="G51" s="89"/>
@@ -4476,13 +4477,13 @@
         <v>0.74</v>
       </c>
       <c r="K51" s="91" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="L51" s="92" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M51" s="96" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="N51" s="93"/>
       <c r="O51" s="94"/>
@@ -4490,16 +4491,16 @@
     </row>
     <row r="52" spans="1:16">
       <c r="A52" s="26" t="s">
+        <v>117</v>
+      </c>
+      <c r="B52" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="C52" s="38" t="s">
         <v>119</v>
       </c>
-      <c r="B52" s="38" t="s">
+      <c r="D52" s="38" t="s">
         <v>120</v>
-      </c>
-      <c r="C52" s="38" t="s">
-        <v>121</v>
-      </c>
-      <c r="D52" s="38" t="s">
-        <v>122</v>
       </c>
       <c r="E52" s="27"/>
       <c r="F52" s="30"/>
@@ -4517,10 +4518,10 @@
         <v>12</v>
       </c>
       <c r="K52" s="36" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="L52" s="33" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="M52" s="34"/>
       <c r="N52" s="34"/>
@@ -4529,16 +4530,16 @@
     </row>
     <row r="53" spans="1:16">
       <c r="A53" s="26" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B53" s="38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C53" s="38" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D53" s="38" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E53" s="27"/>
       <c r="F53" s="30"/>
@@ -4556,10 +4557,10 @@
         <v>0</v>
       </c>
       <c r="K53" s="36" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="L53" s="33" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="M53" s="40"/>
       <c r="N53" s="40"/>
@@ -4568,16 +4569,16 @@
     </row>
     <row r="54" spans="1:16">
       <c r="A54" s="26" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B54" s="38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C54" s="38" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D54" s="38" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E54" s="27"/>
       <c r="F54" s="30"/>
@@ -4595,10 +4596,10 @@
         <v>71</v>
       </c>
       <c r="K54" s="32" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="L54" s="33" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="M54" s="34"/>
       <c r="N54" s="34"/>
@@ -4607,16 +4608,16 @@
     </row>
     <row r="55" spans="1:16">
       <c r="A55" s="26" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B55" s="38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C55" s="38" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="D55" s="38" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E55" s="27"/>
       <c r="F55" s="30"/>
@@ -4634,10 +4635,10 @@
         <v>23</v>
       </c>
       <c r="K55" s="36" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="L55" s="33" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="M55" s="40"/>
       <c r="N55" s="40"/>
@@ -4646,16 +4647,16 @@
     </row>
     <row r="56" spans="1:16">
       <c r="A56" s="26" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B56" s="38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C56" s="38" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D56" s="38" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E56" s="27"/>
       <c r="F56" s="30"/>
@@ -4673,10 +4674,10 @@
         <v>7.5</v>
       </c>
       <c r="K56" s="36" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="L56" s="33" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M56" s="34"/>
       <c r="N56" s="34"/>
@@ -4685,16 +4686,16 @@
     </row>
     <row r="57" spans="1:16">
       <c r="A57" s="26" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B57" s="38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C57" s="38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D57" s="38" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E57" s="27">
         <v>300</v>
@@ -4714,15 +4715,15 @@
         <v>78.39</v>
       </c>
       <c r="K57" s="36" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="L57" s="33" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="M57" s="40"/>
       <c r="N57" s="40"/>
       <c r="O57" s="55" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="P57" s="44" t="s">
         <v>22</v>
@@ -4730,16 +4731,16 @@
     </row>
     <row r="58" spans="1:16">
       <c r="A58" s="26" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B58" s="38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C58" s="38" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D58" s="38" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E58" s="27"/>
       <c r="F58" s="30"/>
@@ -4757,30 +4758,30 @@
         <v>78</v>
       </c>
       <c r="K58" s="36" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="L58" s="33" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M58" s="34"/>
       <c r="N58" s="34"/>
       <c r="O58" s="55" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="P58" s="44"/>
     </row>
     <row r="59" spans="1:16">
       <c r="A59" s="26" t="s">
+        <v>140</v>
+      </c>
+      <c r="B59" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="C59" s="38" t="s">
+        <v>141</v>
+      </c>
+      <c r="D59" s="38" t="s">
         <v>142</v>
-      </c>
-      <c r="B59" s="38" t="s">
-        <v>120</v>
-      </c>
-      <c r="C59" s="38" t="s">
-        <v>143</v>
-      </c>
-      <c r="D59" s="38" t="s">
-        <v>144</v>
       </c>
       <c r="E59" s="27"/>
       <c r="F59" s="30"/>
@@ -4798,10 +4799,10 @@
         <v>20</v>
       </c>
       <c r="K59" s="36" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="L59" s="33" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M59" s="40"/>
       <c r="N59" s="40"/>
@@ -4810,16 +4811,16 @@
     </row>
     <row r="60" spans="1:16" s="4" customFormat="1">
       <c r="A60" s="26" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B60" s="38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C60" s="38" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D60" s="38" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E60" s="27"/>
       <c r="F60" s="30"/>
@@ -4837,7 +4838,7 @@
         <v>2</v>
       </c>
       <c r="K60" s="32" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="L60" s="33"/>
       <c r="M60" s="40"/>
@@ -4847,16 +4848,16 @@
     </row>
     <row r="61" spans="1:16" s="4" customFormat="1">
       <c r="A61" s="26" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B61" s="38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C61" s="38" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D61" s="38" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="E61" s="27"/>
       <c r="F61" s="30"/>
@@ -4874,7 +4875,7 @@
         <v>0</v>
       </c>
       <c r="K61" s="32" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="L61" s="33"/>
       <c r="M61" s="40"/>
@@ -4884,16 +4885,16 @@
     </row>
     <row r="62" spans="1:16">
       <c r="A62" s="26" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B62" s="38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C62" s="38" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D62" s="38" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E62" s="27"/>
       <c r="F62" s="30"/>
@@ -4911,10 +4912,10 @@
         <v>3</v>
       </c>
       <c r="K62" s="32" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="L62" s="33" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="M62" s="34"/>
       <c r="N62" s="34"/>
@@ -4923,16 +4924,16 @@
     </row>
     <row r="63" spans="1:16">
       <c r="A63" s="26" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B63" s="38" t="s">
+        <v>148</v>
+      </c>
+      <c r="C63" s="38" t="s">
+        <v>149</v>
+      </c>
+      <c r="D63" s="38" t="s">
         <v>150</v>
-      </c>
-      <c r="C63" s="38" t="s">
-        <v>151</v>
-      </c>
-      <c r="D63" s="38" t="s">
-        <v>152</v>
       </c>
       <c r="E63" s="27"/>
       <c r="F63" s="30"/>
@@ -4950,10 +4951,10 @@
         <v>85</v>
       </c>
       <c r="K63" s="36" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="L63" s="33" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M63" s="40"/>
       <c r="N63" s="40"/>
@@ -4962,16 +4963,16 @@
     </row>
     <row r="64" spans="1:16">
       <c r="A64" s="26" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B64" s="38" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C64" s="38" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D64" s="38" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E64" s="27"/>
       <c r="F64" s="30"/>
@@ -4989,10 +4990,10 @@
         <v>0</v>
       </c>
       <c r="K64" s="36" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="L64" s="33" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M64" s="34"/>
       <c r="N64" s="34"/>
@@ -5001,16 +5002,16 @@
     </row>
     <row r="65" spans="1:16">
       <c r="A65" s="26" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B65" s="38" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C65" s="38" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D65" s="38" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E65" s="27"/>
       <c r="F65" s="30"/>
@@ -5028,10 +5029,10 @@
         <v>0</v>
       </c>
       <c r="K65" s="36" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="L65" s="33" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M65" s="40"/>
       <c r="N65" s="40"/>
@@ -5040,16 +5041,16 @@
     </row>
     <row r="66" spans="1:16">
       <c r="A66" s="26" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B66" s="38" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C66" s="38" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D66" s="38" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E66" s="27"/>
       <c r="F66" s="30"/>
@@ -5067,10 +5068,10 @@
         <v>0</v>
       </c>
       <c r="K66" s="32" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="L66" s="33" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M66" s="34"/>
       <c r="N66" s="34"/>
@@ -5079,16 +5080,16 @@
     </row>
     <row r="67" spans="1:16">
       <c r="A67" s="26" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="B67" s="38" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C67" s="38" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D67" s="38" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E67" s="27"/>
       <c r="F67" s="30"/>
@@ -5106,10 +5107,10 @@
         <v>70</v>
       </c>
       <c r="K67" s="36" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="L67" s="33" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="M67" s="40"/>
       <c r="N67" s="40"/>
@@ -5118,16 +5119,16 @@
     </row>
     <row r="68" spans="1:16">
       <c r="A68" s="26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B68" s="38" t="s">
+        <v>161</v>
+      </c>
+      <c r="C68" s="38" t="s">
+        <v>162</v>
+      </c>
+      <c r="D68" s="38" t="s">
         <v>163</v>
-      </c>
-      <c r="C68" s="38" t="s">
-        <v>164</v>
-      </c>
-      <c r="D68" s="38" t="s">
-        <v>165</v>
       </c>
       <c r="E68" s="27">
         <v>1000</v>
@@ -5149,10 +5150,10 @@
         <v>59</v>
       </c>
       <c r="K68" s="32" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="L68" s="33" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="M68" s="34"/>
       <c r="N68" s="34"/>
@@ -5161,16 +5162,16 @@
     </row>
     <row r="69" spans="1:16">
       <c r="A69" s="26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B69" s="38" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C69" s="38" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D69" s="38" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E69" s="27"/>
       <c r="F69" s="30"/>
@@ -5188,10 +5189,10 @@
         <v>41</v>
       </c>
       <c r="K69" s="36" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="L69" s="33" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M69" s="40"/>
       <c r="N69" s="40"/>
@@ -5200,16 +5201,16 @@
     </row>
     <row r="70" spans="1:16">
       <c r="A70" s="26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B70" s="38" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C70" s="38" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D70" s="38" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E70" s="27"/>
       <c r="F70" s="30"/>
@@ -5227,10 +5228,10 @@
         <v>30</v>
       </c>
       <c r="K70" s="36" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="L70" s="33" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M70" s="34"/>
       <c r="N70" s="34"/>
@@ -5239,16 +5240,16 @@
     </row>
     <row r="71" spans="1:16">
       <c r="A71" s="26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B71" s="38" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C71" s="38" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D71" s="38" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E71" s="27"/>
       <c r="F71" s="30"/>
@@ -5266,10 +5267,10 @@
         <v>20</v>
       </c>
       <c r="K71" s="36" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="L71" s="33" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M71" s="40"/>
       <c r="N71" s="40"/>
@@ -5278,16 +5279,16 @@
     </row>
     <row r="72" spans="1:16">
       <c r="A72" s="26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B72" s="38" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C72" s="38" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D72" s="38" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E72" s="27">
         <v>200</v>
@@ -5309,10 +5310,10 @@
         <v>48</v>
       </c>
       <c r="K72" s="32" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L72" s="33" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="M72" s="34"/>
       <c r="N72" s="34"/>
@@ -5321,16 +5322,16 @@
     </row>
     <row r="73" spans="1:16">
       <c r="A73" s="26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B73" s="38" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C73" s="38" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D73" s="38" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E73" s="27"/>
       <c r="F73" s="30"/>
@@ -5348,10 +5349,10 @@
         <v>72.5</v>
       </c>
       <c r="K73" s="36" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="L73" s="33" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="M73" s="40"/>
       <c r="N73" s="40"/>
@@ -5360,16 +5361,16 @@
     </row>
     <row r="74" spans="1:16">
       <c r="A74" s="26" t="s">
+        <v>189</v>
+      </c>
+      <c r="B74" s="38" t="s">
+        <v>190</v>
+      </c>
+      <c r="C74" s="38" t="s">
         <v>191</v>
       </c>
-      <c r="B74" s="38" t="s">
+      <c r="D74" s="38" t="s">
         <v>192</v>
-      </c>
-      <c r="C74" s="38" t="s">
-        <v>193</v>
-      </c>
-      <c r="D74" s="38" t="s">
-        <v>194</v>
       </c>
       <c r="E74" s="27"/>
       <c r="F74" s="30"/>
@@ -5387,10 +5388,10 @@
         <v>50</v>
       </c>
       <c r="K74" s="36" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="L74" s="33" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="M74" s="40"/>
       <c r="N74" s="40"/>
@@ -5399,16 +5400,16 @@
     </row>
     <row r="75" spans="1:16">
       <c r="A75" s="26" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B75" s="38" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C75" s="38" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D75" s="38" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E75" s="27"/>
       <c r="F75" s="30"/>
@@ -5426,10 +5427,10 @@
         <v>40</v>
       </c>
       <c r="K75" s="32" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="L75" s="33" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="M75" s="34"/>
       <c r="N75" s="34"/>
@@ -5438,16 +5439,16 @@
     </row>
     <row r="76" spans="1:16">
       <c r="A76" s="26" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B76" s="38" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C76" s="38" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D76" s="38" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E76" s="27"/>
       <c r="F76" s="30"/>
@@ -5465,10 +5466,10 @@
         <v>70</v>
       </c>
       <c r="K76" s="36" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="L76" s="33" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="M76" s="40"/>
       <c r="N76" s="40"/>
@@ -5477,16 +5478,16 @@
     </row>
     <row r="77" spans="1:16">
       <c r="A77" s="26" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B77" s="38" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C77" s="38" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D77" s="38" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E77" s="27"/>
       <c r="F77" s="30"/>
@@ -5504,10 +5505,10 @@
         <v>20</v>
       </c>
       <c r="K77" s="32" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="L77" s="33" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="M77" s="34"/>
       <c r="N77" s="34"/>
@@ -5516,16 +5517,16 @@
     </row>
     <row r="78" spans="1:16">
       <c r="A78" s="26" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B78" s="38" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C78" s="38" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D78" s="38" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E78" s="27"/>
       <c r="F78" s="30"/>
@@ -5543,10 +5544,10 @@
         <v>20</v>
       </c>
       <c r="K78" s="36" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="L78" s="33" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="M78" s="40"/>
       <c r="N78" s="40"/>
@@ -5555,16 +5556,16 @@
     </row>
     <row r="79" spans="1:16">
       <c r="A79" s="26" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="B79" s="38" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C79" s="38" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D79" s="38" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="E79" s="27"/>
       <c r="F79" s="30"/>
@@ -5582,10 +5583,10 @@
         <v>60</v>
       </c>
       <c r="K79" s="36" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="L79" s="33" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="M79" s="34"/>
       <c r="N79" s="34"/>
@@ -5594,16 +5595,16 @@
     </row>
     <row r="80" spans="1:16">
       <c r="A80" s="26" t="s">
+        <v>200</v>
+      </c>
+      <c r="B80" s="38" t="s">
         <v>202</v>
       </c>
-      <c r="B80" s="38" t="s">
-        <v>204</v>
-      </c>
       <c r="C80" s="38" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D80" s="43" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="E80" s="27"/>
       <c r="F80" s="30"/>
@@ -5621,10 +5622,10 @@
         <v>125</v>
       </c>
       <c r="K80" s="36" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="L80" s="33" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="M80" s="40"/>
       <c r="N80" s="40"/>
@@ -5633,16 +5634,16 @@
     </row>
     <row r="81" spans="1:16">
       <c r="A81" s="26" t="s">
+        <v>200</v>
+      </c>
+      <c r="B81" s="38" t="s">
         <v>202</v>
       </c>
-      <c r="B81" s="38" t="s">
-        <v>204</v>
-      </c>
       <c r="C81" s="43" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D81" s="43" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E81" s="27"/>
       <c r="F81" s="30"/>
@@ -5660,10 +5661,10 @@
         <v>25</v>
       </c>
       <c r="K81" s="32" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="L81" s="33" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="M81" s="34"/>
       <c r="N81" s="34"/>
@@ -5675,13 +5676,13 @@
         <v>44</v>
       </c>
       <c r="B82" s="38" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C82" s="38" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D82" s="38" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="E82" s="27">
         <v>350</v>
@@ -5701,10 +5702,10 @@
         <v>10</v>
       </c>
       <c r="K82" s="36" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="L82" s="33" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M82" s="40"/>
       <c r="N82" s="40"/>
@@ -5713,16 +5714,16 @@
     </row>
     <row r="83" spans="1:16">
       <c r="A83" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B83" s="38" t="s">
         <v>24</v>
       </c>
       <c r="C83" s="38" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D83" s="38" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="E83" s="27">
         <v>400</v>
@@ -5742,10 +5743,10 @@
         <v>24</v>
       </c>
       <c r="K83" s="36" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="L83" s="33" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="M83" s="34"/>
       <c r="N83" s="34"/>
@@ -5754,16 +5755,16 @@
     </row>
     <row r="84" spans="1:16">
       <c r="A84" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B84" s="38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C84" s="38" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D84" s="38" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="E84" s="27"/>
       <c r="F84" s="30"/>
@@ -5782,10 +5783,10 @@
         <v>2.2799999999999998</v>
       </c>
       <c r="K84" s="36" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="L84" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M84" s="40">
         <v>7991</v>
@@ -5798,16 +5799,16 @@
     </row>
     <row r="85" spans="1:16">
       <c r="A85" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B85" s="38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C85" s="38" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D85" s="38" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="E85" s="27"/>
       <c r="F85" s="30"/>
@@ -5826,10 +5827,10 @@
         <v>4.51</v>
       </c>
       <c r="K85" s="36" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="L85" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M85" s="34"/>
       <c r="N85" s="34">
@@ -5842,16 +5843,16 @@
     </row>
     <row r="86" spans="1:16">
       <c r="A86" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B86" s="38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C86" s="38" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D86" s="38" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="E86" s="27"/>
       <c r="F86" s="30"/>
@@ -5870,10 +5871,10 @@
         <v>0.49</v>
       </c>
       <c r="K86" s="36" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="L86" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M86" s="40"/>
       <c r="N86" s="40">
@@ -5886,16 +5887,16 @@
     </row>
     <row r="87" spans="1:16">
       <c r="A87" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B87" s="38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C87" s="38" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D87" s="38" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E87" s="27"/>
       <c r="F87" s="30"/>
@@ -5914,10 +5915,10 @@
         <v>0.99</v>
       </c>
       <c r="K87" s="32" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="L87" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M87" s="34"/>
       <c r="N87" s="34">
@@ -5930,16 +5931,16 @@
     </row>
     <row r="88" spans="1:16">
       <c r="A88" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B88" s="38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C88" s="38" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D88" s="38" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="E88" s="27"/>
       <c r="F88" s="30"/>
@@ -5958,10 +5959,10 @@
         <v>5.01</v>
       </c>
       <c r="K88" s="36" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="L88" s="33" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="M88" s="40"/>
       <c r="N88" s="40">
@@ -5974,16 +5975,16 @@
     </row>
     <row r="89" spans="1:16">
       <c r="A89" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B89" s="38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C89" s="38" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D89" s="38" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="E89" s="27"/>
       <c r="F89" s="30"/>
@@ -6002,10 +6003,10 @@
         <v>13.5</v>
       </c>
       <c r="K89" s="32" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="L89" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M89" s="34"/>
       <c r="N89" s="34"/>
@@ -6014,16 +6015,16 @@
     </row>
     <row r="90" spans="1:16">
       <c r="A90" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B90" s="38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C90" s="38" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D90" s="38" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="E90" s="27"/>
       <c r="F90" s="30"/>
@@ -6042,10 +6043,10 @@
         <v>3.62</v>
       </c>
       <c r="K90" s="36" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="L90" s="33" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M90" s="40"/>
       <c r="N90" s="40"/>
@@ -6054,16 +6055,16 @@
     </row>
     <row r="91" spans="1:16">
       <c r="A91" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B91" s="38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C91" s="38" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D91" s="38" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="E91" s="27"/>
       <c r="F91" s="30"/>
@@ -6081,10 +6082,10 @@
         <v>3</v>
       </c>
       <c r="K91" s="36" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="L91" s="33" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="M91" s="34"/>
       <c r="N91" s="34"/>
@@ -6093,16 +6094,16 @@
     </row>
     <row r="92" spans="1:16">
       <c r="A92" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B92" s="38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C92" s="38" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D92" s="38" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E92" s="27"/>
       <c r="F92" s="30"/>
@@ -6121,10 +6122,10 @@
         <v>4.7799999999999994</v>
       </c>
       <c r="K92" s="36" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="L92" s="33" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="M92" s="40"/>
       <c r="N92" s="40"/>
@@ -6135,16 +6136,16 @@
     </row>
     <row r="93" spans="1:16">
       <c r="A93" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B93" s="38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C93" s="38" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D93" s="38" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E93" s="27"/>
       <c r="F93" s="30"/>
@@ -6162,10 +6163,10 @@
         <v>2</v>
       </c>
       <c r="K93" s="32" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="L93" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M93" s="34">
         <v>7991</v>
@@ -6178,16 +6179,16 @@
     </row>
     <row r="94" spans="1:16">
       <c r="A94" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B94" s="38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C94" s="38" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D94" s="38" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="E94" s="27"/>
       <c r="F94" s="30"/>
@@ -6206,10 +6207,10 @@
         <v>2.5</v>
       </c>
       <c r="K94" s="36" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="L94" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M94" s="40">
         <v>7991</v>
@@ -6222,16 +6223,16 @@
     </row>
     <row r="95" spans="1:16">
       <c r="A95" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B95" s="38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C95" s="38" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D95" s="38" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="E95" s="27"/>
       <c r="F95" s="30"/>
@@ -6250,10 +6251,10 @@
         <v>4.3099999999999996</v>
       </c>
       <c r="K95" s="32" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="L95" s="33" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="M95" s="34"/>
       <c r="N95" s="34"/>
@@ -6262,16 +6263,16 @@
     </row>
     <row r="96" spans="1:16">
       <c r="A96" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B96" s="38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C96" s="38" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D96" s="38" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="E96" s="27"/>
       <c r="F96" s="30"/>
@@ -6290,10 +6291,10 @@
         <v>1.72</v>
       </c>
       <c r="K96" s="36" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="L96" s="33" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="M96" s="40"/>
       <c r="N96" s="40"/>
@@ -6302,16 +6303,16 @@
     </row>
     <row r="97" spans="1:26">
       <c r="A97" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B97" s="38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C97" s="38" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D97" s="38" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="E97" s="27"/>
       <c r="F97" s="30"/>
@@ -6330,10 +6331,10 @@
         <v>2.44</v>
       </c>
       <c r="K97" s="36" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="L97" s="33" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="M97" s="34"/>
       <c r="N97" s="34"/>
@@ -6344,16 +6345,16 @@
     </row>
     <row r="98" spans="1:26">
       <c r="A98" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B98" s="38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C98" s="38" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D98" s="38" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="E98" s="27"/>
       <c r="F98" s="30"/>
@@ -6372,10 +6373,10 @@
         <v>2.38</v>
       </c>
       <c r="K98" s="36" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="L98" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M98" s="40"/>
       <c r="N98" s="40"/>
@@ -6386,16 +6387,16 @@
     </row>
     <row r="99" spans="1:26">
       <c r="A99" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B99" s="38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C99" s="38" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D99" s="38" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="E99" s="27"/>
       <c r="F99" s="30"/>
@@ -6414,10 +6415,10 @@
         <v>3.27</v>
       </c>
       <c r="K99" s="32" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="L99" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M99" s="34"/>
       <c r="N99" s="34"/>
@@ -6428,16 +6429,16 @@
     </row>
     <row r="100" spans="1:26">
       <c r="A100" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B100" s="38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C100" s="38" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D100" s="38" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="E100" s="27"/>
       <c r="F100" s="30"/>
@@ -6456,10 +6457,10 @@
         <v>2.57</v>
       </c>
       <c r="K100" s="36" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="L100" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M100" s="40"/>
       <c r="N100" s="40"/>
@@ -6470,16 +6471,16 @@
     </row>
     <row r="101" spans="1:26">
       <c r="A101" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B101" s="38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C101" s="38" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D101" s="38" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="E101" s="27"/>
       <c r="F101" s="30"/>
@@ -6498,10 +6499,10 @@
         <v>2.75</v>
       </c>
       <c r="K101" s="32" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="L101" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M101" s="34">
         <v>912</v>
@@ -6514,16 +6515,16 @@
     </row>
     <row r="102" spans="1:26">
       <c r="A102" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B102" s="38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C102" s="38" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D102" s="38" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E102" s="27"/>
       <c r="F102" s="30"/>
@@ -6542,10 +6543,10 @@
         <v>1.75</v>
       </c>
       <c r="K102" s="36" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="L102" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M102" s="40"/>
       <c r="N102" s="40">
@@ -6558,16 +6559,16 @@
     </row>
     <row r="103" spans="1:26">
       <c r="A103" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B103" s="38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C103" s="38" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D103" s="38" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="E103" s="27"/>
       <c r="F103" s="30"/>
@@ -6585,10 +6586,10 @@
         <v>12</v>
       </c>
       <c r="K103" s="36" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="L103" s="33" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="M103" s="34"/>
       <c r="N103" s="34"/>
@@ -6599,16 +6600,16 @@
     </row>
     <row r="104" spans="1:26">
       <c r="A104" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B104" s="38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C104" s="38" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D104" s="38" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="E104" s="27"/>
       <c r="F104" s="30"/>
@@ -6626,10 +6627,10 @@
         <v>12</v>
       </c>
       <c r="K104" s="36" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="L104" s="33" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="M104" s="40"/>
       <c r="N104" s="40"/>
@@ -6638,16 +6639,16 @@
     </row>
     <row r="105" spans="1:26">
       <c r="A105" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B105" s="38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C105" s="38" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D105" s="38" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="E105" s="27"/>
       <c r="F105" s="30"/>
@@ -6666,10 +6667,10 @@
         <v>3.96</v>
       </c>
       <c r="K105" s="32" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="L105" s="33" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="M105" s="40"/>
       <c r="N105" s="40"/>
@@ -6680,16 +6681,16 @@
     </row>
     <row r="106" spans="1:26" s="4" customFormat="1">
       <c r="A106" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B106" s="38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C106" s="38" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D106" s="38" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="E106" s="27"/>
       <c r="F106" s="30"/>
@@ -6707,10 +6708,10 @@
         <v>4.5</v>
       </c>
       <c r="K106" s="36" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="L106" s="33" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="M106" s="40"/>
       <c r="N106" s="40"/>
@@ -6719,16 +6720,16 @@
     </row>
     <row r="107" spans="1:26">
       <c r="A107" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B107" s="38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C107" s="38" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D107" s="38" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E107" s="27"/>
       <c r="F107" s="30"/>
@@ -6746,30 +6747,30 @@
         <v>0</v>
       </c>
       <c r="K107" s="32" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="L107" s="33" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="M107" s="34"/>
       <c r="N107" s="34"/>
       <c r="O107" s="59"/>
       <c r="P107" s="46" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="108" spans="1:26">
       <c r="A108" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B108" s="38" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C108" s="38" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D108" s="38" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="E108" s="27"/>
       <c r="F108" s="30"/>
@@ -6787,30 +6788,30 @@
         <v>4</v>
       </c>
       <c r="K108" s="36" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="L108" s="33" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="M108" s="34"/>
       <c r="N108" s="34"/>
       <c r="O108" s="59"/>
       <c r="P108" s="46" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="109" spans="1:26">
       <c r="A109" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B109" s="38" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C109" s="38" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D109" s="38" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E109" s="27"/>
       <c r="F109" s="30"/>
@@ -6829,30 +6830,30 @@
         <v>0.87</v>
       </c>
       <c r="K109" s="36" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="L109" s="33" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="M109" s="34"/>
       <c r="N109" s="34"/>
       <c r="O109" s="60"/>
       <c r="P109" s="47" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="110" spans="1:26" s="4" customFormat="1">
       <c r="A110" s="26" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B110" s="38" t="s">
+        <v>292</v>
+      </c>
+      <c r="C110" s="38" t="s">
+        <v>293</v>
+      </c>
+      <c r="D110" s="38" t="s">
         <v>294</v>
-      </c>
-      <c r="C110" s="38" t="s">
-        <v>295</v>
-      </c>
-      <c r="D110" s="38" t="s">
-        <v>296</v>
       </c>
       <c r="E110" s="27"/>
       <c r="F110" s="30"/>
@@ -6870,10 +6871,10 @@
         <v>21.5</v>
       </c>
       <c r="K110" s="36" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="L110" s="33" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="M110" s="34"/>
       <c r="N110" s="34"/>
@@ -6904,7 +6905,7 @@
         <v>5</v>
       </c>
       <c r="C112" s="17" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D112" s="17" t="s">
         <v>6</v>
@@ -6916,7 +6917,7 @@
       <c r="I112" s="18"/>
       <c r="J112" s="64">
         <f>SUM(J19:J111)</f>
-        <v>1870.85</v>
+        <v>1880.85</v>
       </c>
       <c r="K112" s="17"/>
       <c r="L112" s="19"/>
@@ -6949,7 +6950,7 @@
     <hyperlink ref="K19" r:id="rId7" display="Ask for Precision Cut Frame Bundle" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="K20" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="K21" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="K22" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="K22" r:id="rId10" display="Size: 310x310mm" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
     <hyperlink ref="K23" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="K24" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="K25" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>

</xml_diff>